<commit_message>
Added in game spell/belt slot configuration
A nice feature.
</commit_message>
<xml_diff>
--- a/KeyInfo.xlsx
+++ b/KeyInfo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AutoHotkey_1.1.33.10\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA99E45D-AE45-4E10-AFB5-4271BA7205A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98259024-5714-4E6B-BC05-4AB356583567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-2730" windowWidth="21840" windowHeight="38640" xr2:uid="{08B34B33-23F3-4066-BD78-264B39CDC124}"/>
+    <workbookView xWindow="-80" yWindow="-80" windowWidth="38560" windowHeight="21760" xr2:uid="{08B34B33-23F3-4066-BD78-264B39CDC124}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="632" uniqueCount="366">
   <si>
     <t>Keyboard</t>
   </si>
@@ -215,9 +215,6 @@
     <t>Crouch+Attack</t>
   </si>
   <si>
-    <t>Right Item Skill / Ash</t>
-  </si>
-  <si>
     <t>Physics Flask</t>
   </si>
   <si>
@@ -857,9 +854,6 @@
     <t>Cannot change or bind… will open map.</t>
   </si>
   <si>
-    <t>This will break exiting map but I use controller</t>
-  </si>
-  <si>
     <t>PRESS MW</t>
   </si>
   <si>
@@ -878,9 +872,6 @@
     <t>SHIFT-S</t>
   </si>
   <si>
-    <t>Reserved Keys to be mapped to ER settings so shift/ctrl/alt will work on mapped keys</t>
-  </si>
-  <si>
     <t>ER KEY BINDINGS</t>
   </si>
   <si>
@@ -1088,14 +1079,68 @@
     <t>SHIFT-V</t>
   </si>
   <si>
-    <t xml:space="preserve"> NT</t>
+    <t>Reserving for 'm' for map.</t>
+  </si>
+  <si>
+    <t>Available to be used.</t>
+  </si>
+  <si>
+    <t>SHIFT-c</t>
+  </si>
+  <si>
+    <t>Toggle Spell Hand</t>
+  </si>
+  <si>
+    <t>CTRL-SHIFT-z</t>
+  </si>
+  <si>
+    <t>v0.3</t>
+  </si>
+  <si>
+    <t>Toggle Auto-Run</t>
+  </si>
+  <si>
+    <t>SHIFT while moving</t>
+  </si>
+  <si>
+    <t>VERSION</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>v0.1</t>
+  </si>
+  <si>
+    <t>v0.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reserved Keys </t>
+  </si>
+  <si>
+    <t>to be mapped to ER settings so shift/ctrl/alt will work on mapped keys</t>
+  </si>
+  <si>
+    <t>Binding this will break exiting map and menus</t>
+  </si>
+  <si>
+    <t>Set Number of Spell Slots</t>
+  </si>
+  <si>
+    <t>Set Number Belt Slots</t>
+  </si>
+  <si>
+    <t>CTRL-SHIFT-1</t>
+  </si>
+  <si>
+    <t>CTRL-SHIFT-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1146,8 +1191,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1196,6 +1248,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1209,11 +1267,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
@@ -1230,6 +1285,9 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1544,1164 +1602,1428 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3AC6F3-A015-424D-B7A7-C83A7BB3C058}">
-  <dimension ref="A1:H93"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="50.54296875" customWidth="1"/>
-    <col min="3" max="3" width="26.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.7265625" customWidth="1"/>
-    <col min="5" max="5" width="17.1796875" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" customWidth="1"/>
-    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="2" max="2" width="50.54296875" customWidth="1"/>
+    <col min="4" max="4" width="26.54296875" customWidth="1"/>
+    <col min="5" max="5" width="14.7265625" customWidth="1"/>
+    <col min="6" max="6" width="17.1796875" customWidth="1"/>
+    <col min="7" max="7" width="14.7265625" customWidth="1"/>
+    <col min="8" max="8" width="21" customWidth="1"/>
+    <col min="9" max="9" width="41.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B1" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="E1" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="13" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>256</v>
+      </c>
+      <c r="H2" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="I2" s="8" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>357</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="H3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>357</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>357</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>357</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>357</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>357</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>203</v>
+      </c>
+      <c r="I8" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>357</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="G9" s="4"/>
+      <c r="H9" s="2" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>357</v>
+      </c>
+      <c r="B10" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H11" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>357</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="H13" s="2" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>357</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="H14" s="2" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>357</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
+        <v>28</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" t="s">
+        <v>217</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>357</v>
+      </c>
+      <c r="B16" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" t="s">
+        <v>218</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>357</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H18" s="2" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B19" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="10"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="10"/>
+      <c r="H19" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>357</v>
+      </c>
+      <c r="B20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>357</v>
+      </c>
+      <c r="B21" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="H21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>357</v>
+      </c>
+      <c r="B22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22">
+        <v>3</v>
+      </c>
+      <c r="D22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>264</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="H22" s="12" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>357</v>
+      </c>
+      <c r="B23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>37</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H24" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B25" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D25" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="7"/>
+      <c r="H25" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>357</v>
+      </c>
+      <c r="B26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>40</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>357</v>
+      </c>
+      <c r="B27" t="s">
+        <v>41</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+      <c r="D27" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="H27" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>357</v>
+      </c>
+      <c r="B28" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
+      </c>
+      <c r="D28" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="H28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>357</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
+        <v>46</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="H29" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>357</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>48</v>
+      </c>
+      <c r="D30" t="s">
+        <v>49</v>
+      </c>
+      <c r="E30" s="3"/>
+      <c r="F30" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="G30" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="H30" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>357</v>
+      </c>
+      <c r="B31" t="s">
+        <v>50</v>
+      </c>
+      <c r="C31" t="s">
+        <v>51</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="F31" s="4"/>
+      <c r="G31" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="H31" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H32" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B33" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="9"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>357</v>
+      </c>
+      <c r="B34" t="s">
+        <v>76</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="H34" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>357</v>
+      </c>
+      <c r="B35" t="s">
+        <v>58</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="H35" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>357</v>
+      </c>
+      <c r="B36" t="s">
+        <v>75</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H36" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>357</v>
+      </c>
+      <c r="B37" t="s">
+        <v>274</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>358</v>
+      </c>
+      <c r="B38" t="s">
+        <v>313</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="H38" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>357</v>
+      </c>
+      <c r="B39" t="s">
+        <v>259</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="H39" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>357</v>
+      </c>
+      <c r="B40" t="s">
+        <v>260</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="H40" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>357</v>
+      </c>
+      <c r="B41" t="s">
+        <v>53</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="H41" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>357</v>
+      </c>
+      <c r="B42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="H42" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>357</v>
+      </c>
+      <c r="B43" t="s">
+        <v>59</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="H43" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>352</v>
+      </c>
+      <c r="B44" t="s">
+        <v>350</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>351</v>
+      </c>
+      <c r="H44" s="4" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>352</v>
+      </c>
+      <c r="B45" t="s">
+        <v>353</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="H45" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>352</v>
+      </c>
+      <c r="B46" t="s">
+        <v>362</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="H46" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>352</v>
+      </c>
+      <c r="B47" t="s">
+        <v>363</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="H47" s="17" t="s">
+        <v>359</v>
+      </c>
+      <c r="I47" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H48" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B49" s="10" t="s">
+        <v>196</v>
+      </c>
+      <c r="C49" s="10"/>
+      <c r="D49" s="10"/>
+      <c r="E49" s="10"/>
+      <c r="F49" s="10"/>
+      <c r="G49" s="10"/>
+      <c r="H49" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>357</v>
+      </c>
+      <c r="B50" t="s">
+        <v>281</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="H50" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>357</v>
+      </c>
+      <c r="B51" t="s">
+        <v>282</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>357</v>
+      </c>
+      <c r="B52" t="s">
+        <v>283</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>357</v>
+      </c>
+      <c r="B53" t="s">
+        <v>284</v>
+      </c>
+      <c r="E53" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="H53" s="1" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>357</v>
+      </c>
+      <c r="B54" t="s">
+        <v>285</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="H54" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="I54" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>357</v>
+      </c>
+      <c r="B55" t="s">
+        <v>286</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>266</v>
+      </c>
+      <c r="H55" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>357</v>
+      </c>
+      <c r="B56" t="s">
+        <v>287</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>357</v>
+      </c>
+      <c r="B57" t="s">
+        <v>288</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>357</v>
+      </c>
+      <c r="B58" t="s">
+        <v>289</v>
+      </c>
+      <c r="E58" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A59" t="s">
+        <v>357</v>
+      </c>
+      <c r="B59" t="s">
+        <v>290</v>
+      </c>
+      <c r="E59" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="H60" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="I60" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A61" t="s">
+        <v>357</v>
+      </c>
+      <c r="B61" t="s">
+        <v>291</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="H61" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="I61" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A62" t="s">
+        <v>357</v>
+      </c>
+      <c r="B62" t="s">
+        <v>292</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="H62" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A63" t="s">
+        <v>357</v>
+      </c>
+      <c r="B63" t="s">
+        <v>293</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>303</v>
+      </c>
+      <c r="H63" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="E1" s="6"/>
-      <c r="F1" s="14" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2" s="11" t="s">
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" t="s">
+        <v>357</v>
+      </c>
+      <c r="B64" t="s">
+        <v>294</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="H64" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A65" t="s">
+        <v>357</v>
+      </c>
+      <c r="B65" t="s">
+        <v>295</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A66" t="s">
+        <v>357</v>
+      </c>
+      <c r="B66" t="s">
+        <v>296</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="H66" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A67" t="s">
+        <v>357</v>
+      </c>
+      <c r="B67" t="s">
+        <v>297</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>307</v>
+      </c>
+      <c r="H67" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>357</v>
+      </c>
+      <c r="B68" t="s">
+        <v>298</v>
+      </c>
+      <c r="E68" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="H68" s="1" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A69" t="s">
+        <v>357</v>
+      </c>
+      <c r="B69" t="s">
+        <v>299</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A70" t="s">
+        <v>357</v>
+      </c>
+      <c r="B70" t="s">
+        <v>300</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B72" s="10" t="s">
+        <v>197</v>
+      </c>
+      <c r="C72" s="10"/>
+      <c r="D72" s="10"/>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
+      <c r="G72" s="10"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A73" t="s">
+        <v>357</v>
+      </c>
+      <c r="B73" t="s">
+        <v>316</v>
+      </c>
+      <c r="E73" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A74" t="s">
+        <v>357</v>
+      </c>
+      <c r="B74" t="s">
+        <v>317</v>
+      </c>
+      <c r="E74" s="11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A75" t="s">
+        <v>357</v>
+      </c>
+      <c r="B75" t="s">
+        <v>318</v>
+      </c>
+      <c r="E75" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A76" t="s">
+        <v>357</v>
+      </c>
+      <c r="B76" t="s">
+        <v>319</v>
+      </c>
+      <c r="E76" s="11">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A77" t="s">
+        <v>357</v>
+      </c>
+      <c r="B77" t="s">
+        <v>320</v>
+      </c>
+      <c r="E77" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A78" t="s">
+        <v>357</v>
+      </c>
+      <c r="B78" t="s">
+        <v>321</v>
+      </c>
+      <c r="E78" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A79" t="s">
+        <v>357</v>
+      </c>
+      <c r="B79" t="s">
+        <v>322</v>
+      </c>
+      <c r="E79" s="11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A80" t="s">
+        <v>357</v>
+      </c>
+      <c r="B80" t="s">
+        <v>323</v>
+      </c>
+      <c r="E80" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A81" t="s">
+        <v>357</v>
+      </c>
+      <c r="B81" t="s">
+        <v>324</v>
+      </c>
+      <c r="E81" s="11">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A82" t="s">
+        <v>357</v>
+      </c>
+      <c r="B82" t="s">
+        <v>325</v>
+      </c>
+      <c r="E82" s="11">
         <v>0</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="11" t="s">
-        <v>258</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>314</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>257</v>
-      </c>
-      <c r="G2" s="11" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>252</v>
-      </c>
-      <c r="G3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="4"/>
-      <c r="E7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="H8" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="3" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G11" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G12" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="3" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="4"/>
-      <c r="G14" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-      <c r="D15" s="4"/>
-      <c r="G15" s="3" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="4"/>
-      <c r="E16" t="s">
-        <v>218</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D17" s="4"/>
-      <c r="E17" t="s">
-        <v>219</v>
-      </c>
-      <c r="G17" s="3" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18" t="s">
-        <v>26</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G19" s="3" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G20" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A21" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>30</v>
-      </c>
-      <c r="B22">
-        <v>1</v>
-      </c>
-      <c r="C22" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="4"/>
-      <c r="E22" s="3" t="s">
-        <v>278</v>
-      </c>
-      <c r="F22" s="2" t="s">
-        <v>253</v>
-      </c>
-      <c r="G22" s="13" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>32</v>
-      </c>
-      <c r="B23">
-        <v>4</v>
-      </c>
-      <c r="C23" t="s">
-        <v>33</v>
-      </c>
-      <c r="D23" s="4"/>
-      <c r="E23" s="3" t="s">
-        <v>277</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>254</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>34</v>
-      </c>
-      <c r="B24">
-        <v>3</v>
-      </c>
-      <c r="C24" t="s">
-        <v>35</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="G24" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>36</v>
-      </c>
-      <c r="B25">
-        <v>2</v>
-      </c>
-      <c r="C25" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="G25" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G26" s="3" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A27" s="11" t="s">
-        <v>38</v>
-      </c>
-      <c r="B27" s="11" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="8"/>
-      <c r="G27" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>39</v>
-      </c>
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>40</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="F28" s="2" t="s">
-        <v>221</v>
-      </c>
-      <c r="G28" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>41</v>
-      </c>
-      <c r="B29" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G29" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>43</v>
-      </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="F30" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="G30" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>45</v>
-      </c>
-      <c r="B31" t="s">
-        <v>4</v>
-      </c>
-      <c r="C31" t="s">
-        <v>46</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="G31" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>47</v>
-      </c>
-      <c r="B32" t="s">
-        <v>48</v>
-      </c>
-      <c r="C32" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="4"/>
-      <c r="E32" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="F32" s="2" t="s">
-        <v>249</v>
-      </c>
-      <c r="G32" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>50</v>
-      </c>
-      <c r="B33" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" t="s">
-        <v>4</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="E33" s="5"/>
-      <c r="F33" s="2" t="s">
-        <v>350</v>
-      </c>
-      <c r="G33" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G34" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B35" s="10"/>
-      <c r="C35" s="10"/>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" t="s">
-        <v>230</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="G36" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>58</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>76</v>
-      </c>
-      <c r="D38" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G38" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>276</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="G39" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
-        <v>316</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="G40" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
-        <v>260</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="G41" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
-        <v>261</v>
-      </c>
-      <c r="D42" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="G42" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
-        <v>53</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="G43" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
-        <v>59</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="G44" s="5" t="s">
-        <v>240</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G45" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
-        <v>61</v>
-      </c>
-      <c r="D46" s="3" t="s">
-        <v>283</v>
-      </c>
-      <c r="G46" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
-        <v>60</v>
-      </c>
-      <c r="D47" s="3" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="G48" s="1"/>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" s="11" t="s">
-        <v>197</v>
-      </c>
-      <c r="B49" s="11"/>
-      <c r="C49" s="11"/>
-      <c r="D49" s="11"/>
-      <c r="E49" s="11"/>
-      <c r="F49" s="11"/>
-      <c r="G49" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
-        <v>284</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="G50" s="2" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>285</v>
-      </c>
-      <c r="D51" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="G51" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A52" t="s">
-        <v>286</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="G52" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A53" t="s">
-        <v>287</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>212</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
-        <v>288</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="G54" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A55" t="s">
-        <v>289</v>
-      </c>
-      <c r="D55" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A56" t="s">
-        <v>290</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="G56" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="H56" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A57" t="s">
-        <v>291</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A58" t="s">
-        <v>292</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A59" t="s">
-        <v>293</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="G59" s="2" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="G60" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A61" t="s">
-        <v>294</v>
-      </c>
-      <c r="D61" s="3" t="s">
-        <v>304</v>
-      </c>
-      <c r="G61" s="2" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A62" t="s">
-        <v>295</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>305</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A63" t="s">
-        <v>296</v>
-      </c>
-      <c r="D63" s="3" t="s">
-        <v>306</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A64" t="s">
-        <v>297</v>
-      </c>
-      <c r="D64" s="3" t="s">
-        <v>307</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A65" t="s">
-        <v>298</v>
-      </c>
-      <c r="D65" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>299</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A67" t="s">
-        <v>300</v>
-      </c>
-      <c r="D67" s="3" t="s">
-        <v>310</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
-        <v>301</v>
-      </c>
-      <c r="D68" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="G68" s="2" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A69" t="s">
-        <v>302</v>
-      </c>
-      <c r="D69" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
-        <v>303</v>
-      </c>
-      <c r="D70" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A72" s="11" t="s">
-        <v>198</v>
-      </c>
-      <c r="B72" s="11"/>
-      <c r="C72" s="11"/>
-      <c r="D72" s="11"/>
-      <c r="E72" s="11"/>
-      <c r="F72" s="11"/>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
-        <v>319</v>
-      </c>
-      <c r="D73" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A74" t="s">
-        <v>320</v>
-      </c>
-      <c r="D74" s="12">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A75" t="s">
-        <v>321</v>
-      </c>
-      <c r="D75" s="12">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A76" t="s">
-        <v>322</v>
-      </c>
-      <c r="D76" s="12">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A77" t="s">
-        <v>323</v>
-      </c>
-      <c r="D77" s="12">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A78" t="s">
-        <v>324</v>
-      </c>
-      <c r="D78" s="12">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A79" t="s">
-        <v>325</v>
-      </c>
-      <c r="D79" s="12">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A84" t="s">
+        <v>357</v>
+      </c>
+      <c r="B84" t="s">
         <v>326</v>
       </c>
-      <c r="D80" s="12">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A81" t="s">
+      <c r="E84" s="2" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A85" t="s">
+        <v>357</v>
+      </c>
+      <c r="B85" t="s">
         <v>327</v>
       </c>
-      <c r="D81" s="12">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A82" t="s">
+      <c r="E85" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A86" t="s">
+        <v>357</v>
+      </c>
+      <c r="B86" t="s">
         <v>328</v>
       </c>
-      <c r="D82" s="12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A84" t="s">
+      <c r="E86" s="2" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A87" t="s">
+        <v>357</v>
+      </c>
+      <c r="B87" t="s">
         <v>329</v>
       </c>
-      <c r="D84" s="3" t="s">
+      <c r="E87" s="2" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A85" t="s">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A88" t="s">
+        <v>357</v>
+      </c>
+      <c r="B88" t="s">
         <v>330</v>
       </c>
-      <c r="D85" s="3" t="s">
+      <c r="E88" s="2" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86" t="s">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A89" t="s">
+        <v>357</v>
+      </c>
+      <c r="B89" t="s">
         <v>331</v>
       </c>
-      <c r="D86" s="3" t="s">
+      <c r="C89" s="4"/>
+      <c r="D89" s="4"/>
+      <c r="E89" s="2" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A87" t="s">
+      <c r="F89" s="4"/>
+      <c r="G89" s="4"/>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A90" t="s">
+        <v>357</v>
+      </c>
+      <c r="B90" t="s">
         <v>332</v>
       </c>
-      <c r="D87" s="3" t="s">
+      <c r="C90" s="14"/>
+      <c r="D90" s="14"/>
+      <c r="E90" s="2" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+      <c r="F90" s="14"/>
+      <c r="G90" s="14"/>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A91" t="s">
+        <v>357</v>
+      </c>
+      <c r="B91" t="s">
         <v>333</v>
       </c>
-      <c r="D88" s="3" t="s">
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="2" t="s">
         <v>343</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A89" t="s">
+      <c r="F91" s="4"/>
+      <c r="G91" s="4"/>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A92" t="s">
+        <v>357</v>
+      </c>
+      <c r="B92" t="s">
         <v>334</v>
       </c>
-      <c r="B89" s="5"/>
-      <c r="C89" s="5"/>
-      <c r="D89" s="3" t="s">
+      <c r="C92" s="4"/>
+      <c r="D92" s="4"/>
+      <c r="E92" s="2" t="s">
         <v>344</v>
       </c>
-      <c r="E89" s="5"/>
-      <c r="F89" s="5"/>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A90" t="s">
+      <c r="F92" s="4"/>
+      <c r="G92" s="4"/>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A93" t="s">
+        <v>357</v>
+      </c>
+      <c r="B93" t="s">
         <v>335</v>
       </c>
-      <c r="B90" s="15"/>
-      <c r="C90" s="15"/>
-      <c r="D90" s="3" t="s">
+      <c r="E93" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="E90" s="15"/>
-      <c r="F90" s="15"/>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
-        <v>336</v>
-      </c>
-      <c r="B91" s="5"/>
-      <c r="C91" s="5"/>
-      <c r="D91" s="3" t="s">
-        <v>346</v>
-      </c>
-      <c r="E91" s="5"/>
-      <c r="F91" s="5"/>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A92" t="s">
-        <v>337</v>
-      </c>
-      <c r="B92" s="5"/>
-      <c r="C92" s="5"/>
-      <c r="D92" s="3" t="s">
-        <v>347</v>
-      </c>
-      <c r="E92" s="5"/>
-      <c r="F92" s="5"/>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A93" t="s">
-        <v>338</v>
-      </c>
-      <c r="D93" s="3" t="s">
-        <v>348</v>
       </c>
     </row>
   </sheetData>
@@ -2726,1282 +3048,1282 @@
   <sheetData>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="62" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="63" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="178" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="179" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="181" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="182" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="183" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="184" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="185" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="186" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="187" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="188" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="189" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="191" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="192" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="193" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="194" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="195" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A195" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="196" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A196" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="198" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A198" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="199" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A199" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="200" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A200" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="201" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A201" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="202" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A202" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="203" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A203" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="204" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A204" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="206" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A206" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="207" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A207" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="208" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A208" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="209" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A209" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="210" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="211" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A211" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="212" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A212" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="215" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="217" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A217" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="218" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A218" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="219" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="220" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A220" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="221" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="222" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A222" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="223" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="225" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A225" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="226" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="227" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="228" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A228" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="229" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A229" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="230" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A230" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="231" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A231" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="233" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A233" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="234" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A234" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="235" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A235" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="236" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A236" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="237" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A237" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="238" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A238" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="239" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A239" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="241" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A241" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="242" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A242" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="243" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A243" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="244" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A244" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="245" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A245" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="246" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A246" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="247" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A247" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="249" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A249" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="250" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A250" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="251" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A251" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="252" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A252" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="253" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A253" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="254" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A254" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="255" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A255" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="257" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A257" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="258" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A258" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="259" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A259" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="260" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A260" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="261" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A261" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="262" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A262" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="263" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A263" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="266" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A266" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="268" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A268" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="269" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A269" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="270" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A270" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="271" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A271" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="272" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A272" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="273" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A273" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="275" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A275" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="276" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A276" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="277" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A277" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="278" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A278" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="279" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A279" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="280" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A280" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="282" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A282" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="283" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A283" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="284" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A284" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="285" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A285" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="286" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A286" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="287" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A287" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="289" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A289" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="290" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A290" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="291" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A291" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="292" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A292" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="293" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A293" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="294" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A294" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="296" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A296" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="297" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A297" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="298" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A298" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="299" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A299" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="300" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A300" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="301" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A301" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>